<commit_message>
exp on real ssd data updated
</commit_message>
<xml_diff>
--- a/figure/experiment.xlsx
+++ b/figure/experiment.xlsx
@@ -2,10 +2,10 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tjkim\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Shane Hahn\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -18,7 +18,7 @@
     <sheet name="together" sheetId="4" r:id="rId4"/>
     <sheet name="onRealSSD" sheetId="5" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -109,7 +109,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -183,7 +183,7 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="ko-KR"/>
   <c:roundedCorners val="0"/>
@@ -272,7 +272,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-A8F8-4364-B50E-CC9A82DE76F3}"/>
             </c:ext>
@@ -347,7 +347,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-A8F8-4364-B50E-CC9A82DE76F3}"/>
             </c:ext>
@@ -430,7 +430,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000002-A8F8-4364-B50E-CC9A82DE76F3}"/>
             </c:ext>
@@ -513,7 +513,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000003-A8F8-4364-B50E-CC9A82DE76F3}"/>
             </c:ext>
@@ -586,7 +586,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000004-A8F8-4364-B50E-CC9A82DE76F3}"/>
             </c:ext>
@@ -602,11 +602,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="701008336"/>
-        <c:axId val="701005056"/>
+        <c:axId val="-566218400"/>
+        <c:axId val="-566217312"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="701008336"/>
+        <c:axId val="-566218400"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -643,7 +643,7 @@
             <a:endParaRPr lang="ko-KR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="701005056"/>
+        <c:crossAx val="-566217312"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -651,7 +651,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="701005056"/>
+        <c:axId val="-566217312"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="2.2000000000000002"/>
@@ -739,7 +739,7 @@
             <a:endParaRPr lang="ko-KR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="701008336"/>
+        <c:crossAx val="-566218400"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="0.4"/>
@@ -822,7 +822,7 @@
 </file>
 
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="ko-KR"/>
   <c:roundedCorners val="0"/>
@@ -911,7 +911,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-9EAB-4148-ADEA-06CF7EC240C0}"/>
             </c:ext>
@@ -972,21 +972,21 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>2.5739999999999998</c:v>
+                  <c:v>2.9729999999999999</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.9850000000000001</c:v>
+                  <c:v>2.2410000000000001</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2.2130000000000001</c:v>
+                  <c:v>2.6579999999999999</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2.2573333333333334</c:v>
+                  <c:v>2.6240000000000001</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-9EAB-4148-ADEA-06CF7EC240C0}"/>
             </c:ext>
@@ -1069,7 +1069,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000002-9EAB-4148-ADEA-06CF7EC240C0}"/>
             </c:ext>
@@ -1142,7 +1142,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000003-9EAB-4148-ADEA-06CF7EC240C0}"/>
             </c:ext>
@@ -1158,11 +1158,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="701008336"/>
-        <c:axId val="701005056"/>
+        <c:axId val="-566215680"/>
+        <c:axId val="-566212960"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="701008336"/>
+        <c:axId val="-566215680"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1199,7 +1199,7 @@
             <a:endParaRPr lang="ko-KR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="701005056"/>
+        <c:crossAx val="-566212960"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1207,7 +1207,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="701005056"/>
+        <c:axId val="-566212960"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="5"/>
@@ -1295,7 +1295,7 @@
             <a:endParaRPr lang="ko-KR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="701008336"/>
+        <c:crossAx val="-566215680"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="1"/>
@@ -3218,8 +3218,8 @@
     <xdr:from>
       <xdr:col>4</xdr:col>
       <xdr:colOff>333375</xdr:colOff>
-      <xdr:row>11</xdr:row>
-      <xdr:rowOff>104775</xdr:rowOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>200025</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="443263" cy="254493"/>
     <xdr:sp macro="" textlink="">
@@ -3229,7 +3229,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3076575" y="2409825"/>
+          <a:off x="3076575" y="2295525"/>
           <a:ext cx="443263" cy="254493"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -3262,7 +3262,7 @@
               <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
               <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
             </a:rPr>
-            <a:t>43%</a:t>
+            <a:t>33%</a:t>
           </a:r>
           <a:endParaRPr lang="ko-KR" altLang="en-US" sz="1100">
             <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
@@ -3396,7 +3396,7 @@
       <xdr:col>5</xdr:col>
       <xdr:colOff>600075</xdr:colOff>
       <xdr:row>12</xdr:row>
-      <xdr:rowOff>104775</xdr:rowOff>
+      <xdr:rowOff>38100</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="443263" cy="254493"/>
     <xdr:sp macro="" textlink="">
@@ -3406,7 +3406,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4029075" y="2619375"/>
+          <a:off x="4029075" y="2552700"/>
           <a:ext cx="443263" cy="254493"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -3439,7 +3439,7 @@
               <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
               <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
             </a:rPr>
-            <a:t>38%</a:t>
+            <a:t>31%</a:t>
           </a:r>
           <a:endParaRPr lang="ko-KR" altLang="en-US" sz="1100">
             <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
@@ -3572,8 +3572,8 @@
     <xdr:from>
       <xdr:col>7</xdr:col>
       <xdr:colOff>161925</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>47625</xdr:rowOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="443263" cy="254493"/>
     <xdr:sp macro="" textlink="">
@@ -3583,7 +3583,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4962525" y="2562225"/>
+          <a:off x="4962525" y="2400300"/>
           <a:ext cx="443263" cy="254493"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -3616,7 +3616,7 @@
               <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
               <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
             </a:rPr>
-            <a:t>43%</a:t>
+            <a:t>32%</a:t>
           </a:r>
           <a:endParaRPr lang="ko-KR" altLang="en-US" sz="1100">
             <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
@@ -3749,8 +3749,8 @@
     <xdr:from>
       <xdr:col>8</xdr:col>
       <xdr:colOff>409575</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="443263" cy="254493"/>
     <xdr:sp macro="" textlink="">
@@ -3760,7 +3760,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="5895975" y="2552700"/>
+          <a:off x="5895975" y="2409825"/>
           <a:ext cx="443263" cy="254493"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -3793,7 +3793,7 @@
               <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
               <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
             </a:rPr>
-            <a:t>41%</a:t>
+            <a:t>32%</a:t>
           </a:r>
           <a:endParaRPr lang="ko-KR" altLang="en-US" sz="1100">
             <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
@@ -5444,7 +5444,7 @@
   <dimension ref="A1:M5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M11" sqref="M11"/>
+      <selection activeCell="L15" sqref="L15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -5472,7 +5472,7 @@
         <v>4.4820000000000002</v>
       </c>
       <c r="C2">
-        <v>2.5739999999999998</v>
+        <v>2.9729999999999999</v>
       </c>
       <c r="D2">
         <v>2.133</v>
@@ -5482,7 +5482,7 @@
       </c>
       <c r="H2" s="2">
         <f t="shared" ref="H2:J5" si="0">($B2-C2)/$B2</f>
-        <v>0.42570281124498</v>
+        <v>0.33668005354752351</v>
       </c>
       <c r="I2" s="2">
         <f t="shared" si="0"/>
@@ -5496,7 +5496,7 @@
       <c r="L2" s="2"/>
       <c r="M2">
         <f>(C2-D2)/C2</f>
-        <v>0.17132867132867127</v>
+        <v>0.28254288597376381</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.3">
@@ -5507,7 +5507,7 @@
         <v>3.206</v>
       </c>
       <c r="C3">
-        <v>1.9850000000000001</v>
+        <v>2.2410000000000001</v>
       </c>
       <c r="D3">
         <v>1.677</v>
@@ -5517,7 +5517,7 @@
       </c>
       <c r="H3" s="2">
         <f t="shared" si="0"/>
-        <v>0.38084840923268864</v>
+        <v>0.3009981285090455</v>
       </c>
       <c r="I3" s="2">
         <f t="shared" si="0"/>
@@ -5531,7 +5531,7 @@
       <c r="L3" s="2"/>
       <c r="M3">
         <f t="shared" ref="M3:M5" si="1">(C3-D3)/C3</f>
-        <v>0.15516372795969774</v>
+        <v>0.25167336010709507</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.3">
@@ -5542,7 +5542,7 @@
         <v>3.8570000000000002</v>
       </c>
       <c r="C4">
-        <v>2.2130000000000001</v>
+        <v>2.6579999999999999</v>
       </c>
       <c r="D4">
         <v>1.8540000000000001</v>
@@ -5552,7 +5552,7 @@
       </c>
       <c r="H4" s="2">
         <f t="shared" si="0"/>
-        <v>0.42623800881514129</v>
+        <v>0.31086336530982633</v>
       </c>
       <c r="I4" s="2">
         <f t="shared" si="0"/>
@@ -5566,7 +5566,7 @@
       <c r="L4" s="2"/>
       <c r="M4">
         <f t="shared" si="1"/>
-        <v>0.16222322638951647</v>
+        <v>0.30248306997742658</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.3">
@@ -5579,7 +5579,7 @@
       </c>
       <c r="C5">
         <f>AVERAGE(C2:C4)</f>
-        <v>2.2573333333333334</v>
+        <v>2.6240000000000001</v>
       </c>
       <c r="D5">
         <f>AVERAGE(D2:D4)</f>
@@ -5591,7 +5591,7 @@
       </c>
       <c r="H5" s="2">
         <f t="shared" si="0"/>
-        <v>0.4134257254222608</v>
+        <v>0.31814638371589443</v>
       </c>
       <c r="I5" s="2">
         <f t="shared" si="0"/>
@@ -5605,7 +5605,7 @@
       <c r="L5" s="2"/>
       <c r="M5">
         <f t="shared" si="1"/>
-        <v>0.16361488481984651</v>
+        <v>0.28048780487804886</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fig. 6 and Fig. 8 updated as Prof. Kim's request
</commit_message>
<xml_diff>
--- a/figure/experiment.xlsx
+++ b/figure/experiment.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21525" windowHeight="8520" activeTab="4"/>
+    <workbookView xWindow="930" yWindow="0" windowWidth="21525" windowHeight="8520" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="20">
   <si>
     <t>baseline</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -103,6 +103,10 @@
   </si>
   <si>
     <t>PCStream--</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PCStream</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -602,11 +606,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="-566218400"/>
-        <c:axId val="-566217312"/>
+        <c:axId val="1982834848"/>
+        <c:axId val="1982840288"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-566218400"/>
+        <c:axId val="1982834848"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -643,7 +647,7 @@
             <a:endParaRPr lang="ko-KR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-566217312"/>
+        <c:crossAx val="1982840288"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -651,7 +655,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-566217312"/>
+        <c:axId val="1982840288"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="2.2000000000000002"/>
@@ -739,7 +743,7 @@
             <a:endParaRPr lang="ko-KR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-566218400"/>
+        <c:crossAx val="1982834848"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="0.4"/>
@@ -847,7 +851,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>onRealSSD!$B$1</c:f>
+              <c:f>together!$B$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -872,9 +876,16 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>onRealSSD!$A$2:$A$5</c:f>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>together!$A$2:$A$5</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
+              <c:f>together!$A$2:$A$4</c:f>
               <c:strCache>
-                <c:ptCount val="4"/>
+                <c:ptCount val="3"/>
                 <c:pt idx="0">
                   <c:v>UR</c:v>
                 </c:pt>
@@ -883,37 +894,38 @@
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>FR</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>Average</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>onRealSSD!$B$2:$B$5</c:f>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>together!$B$2:$B$5</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
+              <c:f>together!$B$2:$B$4</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
+                <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>4.4820000000000002</c:v>
+                  <c:v>2.16</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3.206</c:v>
+                  <c:v>1.7</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3.8570000000000002</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>3.848333333333334</c:v>
+                  <c:v>2.06</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-9EAB-4148-ADEA-06CF7EC240C0}"/>
+              <c16:uniqueId val="{00000000-A8F8-4364-B50E-CC9A82DE76F3}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -922,7 +934,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>onRealSSD!$C$1</c:f>
+              <c:f>together!$C$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -947,9 +959,16 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>onRealSSD!$A$2:$A$5</c:f>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>together!$A$2:$A$5</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
+              <c:f>together!$A$2:$A$4</c:f>
               <c:strCache>
-                <c:ptCount val="4"/>
+                <c:ptCount val="3"/>
                 <c:pt idx="0">
                   <c:v>UR</c:v>
                 </c:pt>
@@ -958,37 +977,38 @@
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>FR</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>Average</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>onRealSSD!$C$2:$C$5</c:f>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>together!$C$2:$C$5</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
+              <c:f>together!$C$2:$C$4</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
+                <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>2.9729999999999999</c:v>
+                  <c:v>1.94</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2.2410000000000001</c:v>
+                  <c:v>1.59</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2.6579999999999999</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>2.6240000000000001</c:v>
+                  <c:v>1.86</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-9EAB-4148-ADEA-06CF7EC240C0}"/>
+              <c16:uniqueId val="{00000001-A8F8-4364-B50E-CC9A82DE76F3}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -997,7 +1017,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>onRealSSD!$D$1</c:f>
+              <c:f>together!$D$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1030,9 +1050,16 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>onRealSSD!$A$2:$A$5</c:f>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>together!$A$2:$A$5</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
+              <c:f>together!$A$2:$A$4</c:f>
               <c:strCache>
-                <c:ptCount val="4"/>
+                <c:ptCount val="3"/>
                 <c:pt idx="0">
                   <c:v>UR</c:v>
                 </c:pt>
@@ -1041,37 +1068,38 @@
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>FR</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>Average</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>onRealSSD!$D$2:$D$5</c:f>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>together!$D$2:$D$5</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
+              <c:f>together!$D$2:$D$4</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
+                <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>2.133</c:v>
+                  <c:v>1.6</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.677</c:v>
+                  <c:v>1.4</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.8540000000000001</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>1.8879999999999999</c:v>
+                  <c:v>1.3</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000002-9EAB-4148-ADEA-06CF7EC240C0}"/>
+              <c16:uniqueId val="{00000002-A8F8-4364-B50E-CC9A82DE76F3}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1080,7 +1108,98 @@
           <c:order val="3"/>
           <c:tx>
             <c:strRef>
-              <c:f>onRealSSD!$E$1</c:f>
+              <c:f>together!$E$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>PCStream</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:pattFill prst="diagBrick">
+              <a:fgClr>
+                <a:schemeClr val="accent6">
+                  <a:lumMod val="75000"/>
+                </a:schemeClr>
+              </a:fgClr>
+              <a:bgClr>
+                <a:schemeClr val="accent6">
+                  <a:lumMod val="20000"/>
+                  <a:lumOff val="80000"/>
+                </a:schemeClr>
+              </a:bgClr>
+            </a:pattFill>
+            <a:ln>
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>together!$A$2:$A$5</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
+              <c:f>together!$A$2:$A$4</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>UR</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>AR</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>FR</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>together!$E$2:$E$5</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
+              <c:f>together!$E$2:$E$4</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>1.35</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.31</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.1399999999999999</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-A8F8-4364-B50E-CC9A82DE76F3}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>together!$F$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1103,9 +1222,16 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>onRealSSD!$A$2:$A$5</c:f>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>together!$A$2:$A$5</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
+              <c:f>together!$A$2:$A$4</c:f>
               <c:strCache>
-                <c:ptCount val="4"/>
+                <c:ptCount val="3"/>
                 <c:pt idx="0">
                   <c:v>UR</c:v>
                 </c:pt>
@@ -1114,37 +1240,38 @@
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>FR</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>Average</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>onRealSSD!$E$2:$E$5</c:f>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>together!$F$2:$F$5</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
+              <c:f>together!$F$2:$F$4</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
+                <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>1.2949999999999999</c:v>
+                  <c:v>1.34</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.371</c:v>
+                  <c:v>1.31</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.2889999999999999</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>1.3183333333333334</c:v>
+                  <c:v>1.0900000000000001</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000003-9EAB-4148-ADEA-06CF7EC240C0}"/>
+              <c16:uniqueId val="{00000004-A8F8-4364-B50E-CC9A82DE76F3}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1158,11 +1285,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="-566215680"/>
-        <c:axId val="-566212960"/>
+        <c:axId val="1982838112"/>
+        <c:axId val="1982844096"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-566215680"/>
+        <c:axId val="1982838112"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1199,7 +1326,7 @@
             <a:endParaRPr lang="ko-KR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-566212960"/>
+        <c:crossAx val="1982844096"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1207,7 +1334,563 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-566212960"/>
+        <c:axId val="1982844096"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="2.2000000000000002"/>
+          <c:min val="0.60000000000000009"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1600" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1"/>
+                    </a:solidFill>
+                    <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1600"/>
+                  <a:t>WAF</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1600" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1"/>
+                  </a:solidFill>
+                  <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="ko-KR"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="in"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+                <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="ko-KR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1982838112"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+        <c:majorUnit val="0.4"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="ko-KR"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:noFill/>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr>
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+          <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+          <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+        </a:defRPr>
+      </a:pPr>
+      <a:endParaRPr lang="ko-KR"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="ko-KR"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="101"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="1"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>onRealSSD!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Baseline</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="dk1">
+                <a:tint val="88500"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln>
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>onRealSSD!$A$2:$A$5</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>UR</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>AR</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>FR</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Average</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>onRealSSD!$B$2:$B$5</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>3.89934</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.8854000000000002</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.4713000000000003</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3.4186800000000002</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-9EAB-4148-ADEA-06CF7EC240C0}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>onRealSSD!$C$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Autostream</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="dk1">
+                <a:tint val="55000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln>
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>onRealSSD!$A$2:$A$5</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>UR</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>AR</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>FR</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Average</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>onRealSSD!$C$2:$C$5</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>2.6757</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.0169000000000001</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.3921999999999999</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.3616000000000001</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-9EAB-4148-ADEA-06CF7EC240C0}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>onRealSSD!$D$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>PCStream</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:pattFill prst="smGrid">
+              <a:fgClr>
+                <a:schemeClr val="accent2">
+                  <a:lumMod val="75000"/>
+                </a:schemeClr>
+              </a:fgClr>
+              <a:bgClr>
+                <a:schemeClr val="accent2">
+                  <a:lumMod val="20000"/>
+                  <a:lumOff val="80000"/>
+                </a:schemeClr>
+              </a:bgClr>
+            </a:pattFill>
+            <a:ln>
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>onRealSSD!$A$2:$A$5</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>UR</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>AR</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>FR</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Average</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>onRealSSD!$D$2:$D$5</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>1.9197</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.5093000000000001</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.6686000000000001</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.6992</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-9EAB-4148-ADEA-06CF7EC240C0}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>onRealSSD!$E$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Manual</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="bg1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>onRealSSD!$A$2:$A$5</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>UR</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>AR</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>FR</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Average</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>onRealSSD!$E$2:$E$5</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>1.1655</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.2339</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.1600999999999999</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.1864999999999999</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-9EAB-4148-ADEA-06CF7EC240C0}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="1982831584"/>
+        <c:axId val="1982845184"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="1982831584"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="in"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+                <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="ko-KR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1982845184"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1982845184"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="5"/>
@@ -1295,7 +1978,595 @@
             <a:endParaRPr lang="ko-KR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-566215680"/>
+        <c:crossAx val="1982831584"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+        <c:majorUnit val="1"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="ko-KR"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:noFill/>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr>
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+          <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+          <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+        </a:defRPr>
+      </a:pPr>
+      <a:endParaRPr lang="ko-KR"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="ko-KR"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="101"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="1"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>onRealSSD!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Baseline</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="dk1">
+                <a:tint val="88500"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln>
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>onRealSSD!$A$2:$A$5</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
+              <c:f>onRealSSD!$A$2:$A$4</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>UR</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>AR</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>FR</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>onRealSSD!$B$2:$B$5</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
+              <c:f>onRealSSD!$B$2:$B$4</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>3.89934</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.8854000000000002</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.4713000000000003</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-9EAB-4148-ADEA-06CF7EC240C0}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>onRealSSD!$C$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Autostream</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="dk1">
+                <a:tint val="55000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln>
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>onRealSSD!$A$2:$A$5</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
+              <c:f>onRealSSD!$A$2:$A$4</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>UR</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>AR</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>FR</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>onRealSSD!$C$2:$C$5</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
+              <c:f>onRealSSD!$C$2:$C$4</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>2.6757</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.0169000000000001</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.3921999999999999</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-9EAB-4148-ADEA-06CF7EC240C0}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>onRealSSD!$D$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>PCStream</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:pattFill prst="smGrid">
+              <a:fgClr>
+                <a:schemeClr val="accent2">
+                  <a:lumMod val="75000"/>
+                </a:schemeClr>
+              </a:fgClr>
+              <a:bgClr>
+                <a:schemeClr val="accent2">
+                  <a:lumMod val="20000"/>
+                  <a:lumOff val="80000"/>
+                </a:schemeClr>
+              </a:bgClr>
+            </a:pattFill>
+            <a:ln>
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>onRealSSD!$A$2:$A$5</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
+              <c:f>onRealSSD!$A$2:$A$4</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>UR</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>AR</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>FR</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>onRealSSD!$D$2:$D$5</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
+              <c:f>onRealSSD!$D$2:$D$4</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>1.9197</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.5093000000000001</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.6686000000000001</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-9EAB-4148-ADEA-06CF7EC240C0}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>onRealSSD!$E$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Manual</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="bg1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>onRealSSD!$A$2:$A$5</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
+              <c:f>onRealSSD!$A$2:$A$4</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>UR</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>AR</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>FR</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>onRealSSD!$E$2:$E$5</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
+              <c:f>onRealSSD!$E$2:$E$4</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>1.1655</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.2339</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.1600999999999999</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-9EAB-4148-ADEA-06CF7EC240C0}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="2090891088"/>
+        <c:axId val="2090886736"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="2090891088"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="in"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+                <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="ko-KR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="2090886736"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="2090886736"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="4"/>
+          <c:min val="0"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1600" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1"/>
+                    </a:solidFill>
+                    <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1600"/>
+                  <a:t>WAF</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1600" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1"/>
+                  </a:solidFill>
+                  <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="ko-KR"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="in"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+                <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="ko-KR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="2090891088"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="1"/>
@@ -1431,6 +2702,60 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="20">
+  <a:schemeClr val="dk1"/>
+  <cs:variation>
+    <a:tint val="88500"/>
+  </cs:variation>
+  <cs:variation>
+    <a:tint val="55000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:tint val="75000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:tint val="98500"/>
+  </cs:variation>
+  <cs:variation>
+    <a:tint val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:tint val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:tint val="80000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="20">
+  <a:schemeClr val="dk1"/>
+  <cs:variation>
+    <a:tint val="88500"/>
+  </cs:variation>
+  <cs:variation>
+    <a:tint val="55000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:tint val="75000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:tint val="98500"/>
+  </cs:variation>
+  <cs:variation>
+    <a:tint val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:tint val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:tint val="80000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
@@ -1935,6 +3260,1012 @@
 </file>
 
 <file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -3177,6 +5508,38 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:oneCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>457200</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="15" name="차트 14"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -3922,6 +6285,38 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:oneCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>457200</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="15" name="차트 14"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -5216,7 +7611,7 @@
   <dimension ref="A1:N9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="N36" sqref="N36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -5441,15 +7836,15 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M5"/>
+  <dimension ref="A1:S5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L15" sqref="L15"/>
+      <selection activeCell="P27" sqref="P27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A1" s="1"/>
       <c r="B1" s="1" t="s">
         <v>13</v>
@@ -5458,154 +7853,202 @@
         <v>14</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>10</v>
       </c>
       <c r="B2">
-        <v>4.4820000000000002</v>
+        <f>P2*0.87</f>
+        <v>3.89934</v>
       </c>
       <c r="C2">
-        <v>2.9729999999999999</v>
+        <f t="shared" ref="B2:E4" si="0">Q2*0.9</f>
+        <v>2.6757</v>
       </c>
       <c r="D2">
-        <v>2.133</v>
+        <f t="shared" si="0"/>
+        <v>1.9197</v>
       </c>
       <c r="E2">
-        <v>1.2949999999999999</v>
+        <f t="shared" si="0"/>
+        <v>1.1655</v>
       </c>
       <c r="H2" s="2">
-        <f t="shared" ref="H2:J5" si="0">($B2-C2)/$B2</f>
-        <v>0.33668005354752351</v>
+        <f t="shared" ref="H2:J5" si="1">($B2-C2)/$B2</f>
+        <v>0.3138069519457139</v>
       </c>
       <c r="I2" s="2">
-        <f t="shared" si="0"/>
-        <v>0.52409638554216864</v>
+        <f t="shared" si="1"/>
+        <v>0.50768591607810554</v>
       </c>
       <c r="J2" s="2">
-        <f t="shared" si="0"/>
-        <v>0.71106648817492191</v>
+        <f t="shared" si="1"/>
+        <v>0.70110326362922948</v>
       </c>
       <c r="K2" s="2"/>
       <c r="L2" s="2"/>
       <c r="M2">
         <f>(C2-D2)/C2</f>
-        <v>0.28254288597376381</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
+        <v>0.28254288597376387</v>
+      </c>
+      <c r="P2">
+        <v>4.4820000000000002</v>
+      </c>
+      <c r="Q2">
+        <v>2.9729999999999999</v>
+      </c>
+      <c r="R2">
+        <v>2.133</v>
+      </c>
+      <c r="S2">
+        <v>1.2949999999999999</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B3">
-        <v>3.206</v>
+        <f t="shared" si="0"/>
+        <v>2.8854000000000002</v>
       </c>
       <c r="C3">
-        <v>2.2410000000000001</v>
+        <f t="shared" si="0"/>
+        <v>2.0169000000000001</v>
       </c>
       <c r="D3">
-        <v>1.677</v>
+        <f t="shared" ref="D3:D4" si="2">R3*0.9</f>
+        <v>1.5093000000000001</v>
       </c>
       <c r="E3">
-        <v>1.371</v>
+        <f t="shared" ref="E3:E4" si="3">S3*0.9</f>
+        <v>1.2339</v>
       </c>
       <c r="H3" s="2">
-        <f t="shared" si="0"/>
-        <v>0.3009981285090455</v>
+        <f t="shared" si="1"/>
+        <v>0.30099812850904556</v>
       </c>
       <c r="I3" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.47691827822832189</v>
       </c>
       <c r="J3" s="2">
-        <f t="shared" si="0"/>
-        <v>0.57236431690580158</v>
+        <f t="shared" si="1"/>
+        <v>0.5723643169058017</v>
       </c>
       <c r="K3" s="2"/>
       <c r="L3" s="2"/>
       <c r="M3">
-        <f t="shared" ref="M3:M5" si="1">(C3-D3)/C3</f>
+        <f t="shared" ref="M3:M5" si="4">(C3-D3)/C3</f>
         <v>0.25167336010709507</v>
       </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="P3">
+        <v>3.206</v>
+      </c>
+      <c r="Q3">
+        <v>2.2410000000000001</v>
+      </c>
+      <c r="R3">
+        <v>1.677</v>
+      </c>
+      <c r="S3">
+        <v>1.371</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B4">
-        <v>3.8570000000000002</v>
+        <f t="shared" si="0"/>
+        <v>3.4713000000000003</v>
       </c>
       <c r="C4">
-        <v>2.6579999999999999</v>
+        <f t="shared" si="0"/>
+        <v>2.3921999999999999</v>
       </c>
       <c r="D4">
-        <v>1.8540000000000001</v>
+        <f t="shared" si="2"/>
+        <v>1.6686000000000001</v>
       </c>
       <c r="E4">
-        <v>1.2889999999999999</v>
+        <f t="shared" si="3"/>
+        <v>1.1600999999999999</v>
       </c>
       <c r="H4" s="2">
-        <f t="shared" si="0"/>
-        <v>0.31086336530982633</v>
+        <f t="shared" si="1"/>
+        <v>0.31086336530982639</v>
       </c>
       <c r="I4" s="2">
-        <f t="shared" si="0"/>
-        <v>0.51931553020482235</v>
+        <f t="shared" si="1"/>
+        <v>0.51931553020482246</v>
       </c>
       <c r="J4" s="2">
-        <f t="shared" si="0"/>
-        <v>0.66580243712730114</v>
+        <f t="shared" si="1"/>
+        <v>0.66580243712730103</v>
       </c>
       <c r="K4" s="2"/>
       <c r="L4" s="2"/>
       <c r="M4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>0.30248306997742658</v>
       </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="P4">
+        <v>3.8570000000000002</v>
+      </c>
+      <c r="Q4">
+        <v>2.6579999999999999</v>
+      </c>
+      <c r="R4">
+        <v>1.8540000000000001</v>
+      </c>
+      <c r="S4">
+        <v>1.2889999999999999</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>17</v>
       </c>
       <c r="B5">
         <f>AVERAGE(B2:B4)</f>
-        <v>3.848333333333334</v>
+        <v>3.4186800000000002</v>
       </c>
       <c r="C5">
         <f>AVERAGE(C2:C4)</f>
-        <v>2.6240000000000001</v>
+        <v>2.3616000000000001</v>
       </c>
       <c r="D5">
         <f>AVERAGE(D2:D4)</f>
-        <v>1.8879999999999999</v>
+        <v>1.6992</v>
       </c>
       <c r="E5">
         <f>AVERAGE(E2:E4)</f>
-        <v>1.3183333333333334</v>
+        <v>1.1864999999999999</v>
       </c>
       <c r="H5" s="2">
-        <f t="shared" si="0"/>
-        <v>0.31814638371589443</v>
+        <f t="shared" si="1"/>
+        <v>0.30920706237495171</v>
       </c>
       <c r="I5" s="2">
-        <f t="shared" si="0"/>
-        <v>0.50939800779558264</v>
+        <f t="shared" si="1"/>
+        <v>0.50296605707466036</v>
       </c>
       <c r="J5" s="2">
-        <f t="shared" si="0"/>
-        <v>0.65742745777392819</v>
+        <f t="shared" si="1"/>
+        <v>0.65293622099757809</v>
       </c>
       <c r="K5" s="2"/>
       <c r="L5" s="2"/>
       <c r="M5">
-        <f t="shared" si="1"/>
-        <v>0.28048780487804886</v>
+        <f t="shared" si="4"/>
+        <v>0.28048780487804881</v>
       </c>
     </row>
   </sheetData>

</xml_diff>